<commit_message>
All models complete, starting flight tests.
</commit_message>
<xml_diff>
--- a/models/mini_fixedwing_14/team14.xlsx
+++ b/models/mini_fixedwing_14/team14.xlsx
@@ -593,7 +593,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,6 +622,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4285F4"/>
         <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -659,7 +665,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -724,6 +730,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -733,6 +743,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -817,7 +831,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF4285F4"/>
       <rgbColor rgb="FF46BDC6"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -847,9 +861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>235800</xdr:colOff>
+      <xdr:colOff>235440</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -863,7 +877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11103480" y="7153200"/>
-          <a:ext cx="6114600" cy="3790440"/>
+          <a:ext cx="6114240" cy="3790080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -884,9 +898,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>350280</xdr:colOff>
+      <xdr:colOff>349920</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -900,7 +914,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11103480" y="4248360"/>
-          <a:ext cx="6229080" cy="2676240"/>
+          <a:ext cx="6228720" cy="2675880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -922,8 +936,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="B40 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1838,7 +1852,7 @@
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="16" t="n">
         <v>0.004</v>
       </c>
       <c r="C26" s="2"/>
@@ -2331,7 +2345,7 @@
       <c r="A40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="9" t="n">
+      <c r="B40" s="16" t="n">
         <v>0.004</v>
       </c>
       <c r="C40" s="2"/>
@@ -2888,7 +2902,7 @@
       <c r="G56" s="14" t="n">
         <v>1E-006</v>
       </c>
-      <c r="K56" s="16" t="s">
+      <c r="K56" s="17" t="s">
         <v>62</v>
       </c>
       <c r="N56" s="2"/>
@@ -2917,7 +2931,7 @@
       <c r="E57" s="5"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="K57" s="16" t="s">
+      <c r="K57" s="17" t="s">
         <v>64</v>
       </c>
       <c r="N57" s="2"/>
@@ -2946,7 +2960,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="K58" s="17"/>
+      <c r="K58" s="18"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -3030,7 +3044,7 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="18" t="n">
+      <c r="B62" s="19" t="n">
         <v>0.0254</v>
       </c>
       <c r="N62" s="2"/>
@@ -3228,7 +3242,7 @@
       <c r="A68" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="9" t="n">
+      <c r="B68" s="16" t="n">
         <v>0.001438</v>
       </c>
       <c r="C68" s="2"/>
@@ -3716,7 +3730,7 @@
       <c r="A82" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="9" t="n">
+      <c r="B82" s="16" t="n">
         <v>0.005681</v>
       </c>
       <c r="C82" s="2"/>
@@ -3928,7 +3942,7 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="16" t="s">
+      <c r="A89" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B89" s="9" t="s">
@@ -4153,7 +4167,7 @@
       <c r="A96" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B96" s="9" t="n">
+      <c r="B96" s="16" t="n">
         <v>0.004233</v>
       </c>
       <c r="C96" s="2"/>
@@ -4364,7 +4378,7 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="16" t="s">
+      <c r="A103" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B103" s="9" t="s">
@@ -4547,7 +4561,7 @@
       <c r="A109" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B109" s="9" t="n">
+      <c r="B109" s="16" t="n">
         <v>0.4753</v>
       </c>
       <c r="C109" s="9" t="n">
@@ -4780,7 +4794,7 @@
       <c r="Z116" s="2"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="16" t="s">
+      <c r="A117" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B117" s="9" t="s">
@@ -4845,7 +4859,7 @@
       <c r="A120" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B120" s="9" t="n">
+      <c r="B120" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C120" s="2"/>
@@ -4877,7 +4891,7 @@
       <c r="A121" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B121" s="19" t="n">
+      <c r="B121" s="20" t="n">
         <v>5.73</v>
       </c>
       <c r="C121" s="2"/>
@@ -4909,7 +4923,7 @@
       <c r="A122" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B122" s="19" t="n">
+      <c r="B122" s="20" t="n">
         <v>0.6016</v>
       </c>
       <c r="C122" s="2"/>
@@ -4941,7 +4955,7 @@
       <c r="A123" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B123" s="19" t="n">
+      <c r="B123" s="20" t="n">
         <v>0.1718</v>
       </c>
       <c r="C123" s="2"/>
@@ -4973,7 +4987,7 @@
       <c r="A124" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B124" s="19" t="n">
+      <c r="B124" s="20" t="n">
         <v>0.1047</v>
       </c>
       <c r="C124" s="2"/>
@@ -5005,7 +5019,7 @@
       <c r="A125" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B125" s="19" t="n">
+      <c r="B125" s="20" t="n">
         <v>-8.59</v>
       </c>
       <c r="C125" s="2"/>
@@ -5037,7 +5051,7 @@
       <c r="A126" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B126" s="19" t="n">
+      <c r="B126" s="20" t="n">
         <v>-0.802</v>
       </c>
       <c r="C126" s="2"/>
@@ -5069,7 +5083,7 @@
       <c r="A127" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B127" s="9" t="n">
+      <c r="B127" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C127" s="2"/>
@@ -5101,7 +5115,7 @@
       <c r="A128" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B128" s="9" t="n">
+      <c r="B128" s="16" t="n">
         <v>-0.42</v>
       </c>
       <c r="C128" s="9" t="n">
@@ -5137,7 +5151,7 @@
       <c r="A129" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B129" s="19" t="n">
+      <c r="B129" s="20" t="n">
         <v>0.0103</v>
       </c>
       <c r="C129" s="2"/>
@@ -5169,7 +5183,7 @@
       <c r="A130" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B130" s="9" t="n">
+      <c r="B130" s="16" t="n">
         <v>1</v>
       </c>
       <c r="C130" s="9" t="n">
@@ -5205,7 +5219,7 @@
       <c r="A131" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B131" s="9" t="n">
+      <c r="B131" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C131" s="9" t="n">
@@ -5241,7 +5255,7 @@
       <c r="A132" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B132" s="9" t="n">
+      <c r="B132" s="16" t="n">
         <v>4</v>
       </c>
       <c r="C132" s="2"/>
@@ -5322,7 +5336,7 @@
       <c r="A135" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B135" s="9" t="n">
+      <c r="B135" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C135" s="2"/>
@@ -5352,7 +5366,7 @@
       <c r="A136" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B136" s="19" t="n">
+      <c r="B136" s="20" t="n">
         <v>5.73</v>
       </c>
       <c r="C136" s="2"/>
@@ -5382,7 +5396,7 @@
       <c r="A137" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B137" s="19" t="n">
+      <c r="B137" s="20" t="n">
         <v>0.6016</v>
       </c>
       <c r="C137" s="2"/>
@@ -5412,7 +5426,7 @@
       <c r="A138" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B138" s="19" t="n">
+      <c r="B138" s="20" t="n">
         <v>0.1718</v>
       </c>
       <c r="C138" s="2"/>
@@ -5442,7 +5456,7 @@
       <c r="A139" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B139" s="19" t="n">
+      <c r="B139" s="20" t="n">
         <v>0.1047</v>
       </c>
       <c r="C139" s="2"/>
@@ -5470,7 +5484,7 @@
       <c r="A140" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B140" s="19" t="n">
+      <c r="B140" s="20" t="n">
         <v>-8.59</v>
       </c>
       <c r="C140" s="2"/>
@@ -5500,7 +5514,7 @@
       <c r="A141" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B141" s="19" t="n">
+      <c r="B141" s="20" t="n">
         <v>-0.802</v>
       </c>
       <c r="C141" s="2"/>
@@ -5530,7 +5544,7 @@
       <c r="A142" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B142" s="9" t="n">
+      <c r="B142" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C142" s="2"/>
@@ -5560,7 +5574,7 @@
       <c r="A143" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B143" s="9" t="n">
+      <c r="B143" s="16" t="n">
         <v>-0.4</v>
       </c>
       <c r="C143" s="9" t="n">
@@ -5594,7 +5608,7 @@
       <c r="A144" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B144" s="19" t="n">
+      <c r="B144" s="20" t="n">
         <v>0.0297</v>
       </c>
       <c r="C144" s="2"/>
@@ -5624,7 +5638,7 @@
       <c r="A145" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B145" s="9" t="n">
+      <c r="B145" s="16" t="n">
         <v>1</v>
       </c>
       <c r="C145" s="9" t="n">
@@ -5658,7 +5672,7 @@
       <c r="A146" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B146" s="9" t="n">
+      <c r="B146" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C146" s="9" t="n">
@@ -5692,7 +5706,7 @@
       <c r="A147" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B147" s="9" t="n">
+      <c r="B147" s="16" t="n">
         <v>-4</v>
       </c>
       <c r="C147" s="2"/>
@@ -5763,7 +5777,7 @@
       <c r="A150" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B150" s="19" t="n">
+      <c r="B150" s="20" t="n">
         <v>0.1047</v>
       </c>
       <c r="C150" s="2"/>
@@ -5794,7 +5808,7 @@
       <c r="A151" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B151" s="19" t="n">
+      <c r="B151" s="20" t="n">
         <v>4.8128</v>
       </c>
       <c r="C151" s="2"/>
@@ -5825,7 +5839,7 @@
       <c r="A152" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B152" s="19" t="n">
+      <c r="B152" s="20" t="n">
         <v>0.4584</v>
       </c>
       <c r="C152" s="2"/>
@@ -5856,7 +5870,7 @@
       <c r="A153" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B153" s="19" t="n">
+      <c r="B153" s="20" t="n">
         <v>-0.54677</v>
       </c>
       <c r="C153" s="2"/>
@@ -5887,7 +5901,7 @@
       <c r="A154" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B154" s="19" t="n">
+      <c r="B154" s="20" t="n">
         <v>0.34301</v>
       </c>
       <c r="C154" s="2"/>
@@ -5917,7 +5931,7 @@
       <c r="A155" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B155" s="19" t="n">
+      <c r="B155" s="20" t="n">
         <v>-3.6211</v>
       </c>
       <c r="C155" s="2"/>
@@ -5947,7 +5961,7 @@
       <c r="A156" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B156" s="19" t="n">
+      <c r="B156" s="20" t="n">
         <v>-0.9033</v>
       </c>
       <c r="C156" s="2"/>
@@ -5977,7 +5991,7 @@
       <c r="A157" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B157" s="9" t="n">
+      <c r="B157" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C157" s="2"/>
@@ -6007,10 +6021,10 @@
       <c r="A158" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B158" s="19" t="n">
+      <c r="B158" s="20" t="n">
         <v>0.5256276</v>
       </c>
-      <c r="C158" s="19" t="n">
+      <c r="C158" s="21" t="n">
         <v>0.2286</v>
       </c>
       <c r="D158" s="9" t="n">
@@ -6041,7 +6055,7 @@
       <c r="A159" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B159" s="19" t="n">
+      <c r="B159" s="20" t="n">
         <v>0.06967</v>
       </c>
       <c r="C159" s="2"/>
@@ -6071,7 +6085,7 @@
       <c r="A160" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B160" s="9" t="n">
+      <c r="B160" s="16" t="n">
         <v>1</v>
       </c>
       <c r="C160" s="9" t="n">
@@ -6105,7 +6119,7 @@
       <c r="A161" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B161" s="9" t="n">
+      <c r="B161" s="16" t="n">
         <v>0</v>
       </c>
       <c r="C161" s="9" t="n">
@@ -6139,7 +6153,7 @@
       <c r="A162" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B162" s="9" t="n">
+      <c r="B162" s="16" t="n">
         <v>-2</v>
       </c>
       <c r="C162" s="2"/>
@@ -6212,7 +6226,7 @@
       <c r="A165" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B165" s="19" t="n">
+      <c r="B165" s="21" t="n">
         <v>0.1047</v>
       </c>
       <c r="C165" s="2"/>
@@ -6243,7 +6257,7 @@
       <c r="A166" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B166" s="19" t="n">
+      <c r="B166" s="21" t="n">
         <v>4.8128</v>
       </c>
       <c r="C166" s="2"/>
@@ -6274,7 +6288,7 @@
       <c r="A167" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B167" s="19" t="n">
+      <c r="B167" s="21" t="n">
         <v>0.4584</v>
       </c>
       <c r="C167" s="2"/>
@@ -6305,7 +6319,7 @@
       <c r="A168" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B168" s="19" t="n">
+      <c r="B168" s="21" t="n">
         <v>-0.54677</v>
       </c>
       <c r="C168" s="2"/>
@@ -6336,7 +6350,7 @@
       <c r="A169" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B169" s="19" t="n">
+      <c r="B169" s="21" t="n">
         <v>0.34301</v>
       </c>
       <c r="C169" s="2"/>
@@ -6366,7 +6380,7 @@
       <c r="A170" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B170" s="19" t="n">
+      <c r="B170" s="21" t="n">
         <v>-3.6211</v>
       </c>
       <c r="C170" s="2"/>
@@ -6396,7 +6410,7 @@
       <c r="A171" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B171" s="19" t="n">
+      <c r="B171" s="21" t="n">
         <v>-0.9033</v>
       </c>
       <c r="C171" s="2"/>
@@ -6456,10 +6470,10 @@
       <c r="A173" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B173" s="19" t="n">
+      <c r="B173" s="21" t="n">
         <v>0.5256276</v>
       </c>
-      <c r="C173" s="19" t="n">
+      <c r="C173" s="21" t="n">
         <v>-0.2286</v>
       </c>
       <c r="D173" s="9" t="n">
@@ -6490,7 +6504,7 @@
       <c r="A174" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B174" s="19" t="n">
+      <c r="B174" s="21" t="n">
         <v>0.06967</v>
       </c>
       <c r="C174" s="2"/>
@@ -6690,22 +6704,22 @@
       <c r="Z180" s="2"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="20" t="s">
+      <c r="A181" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B181" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C181" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D181" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E181" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F181" s="21" t="n">
+      <c r="B181" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C181" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" s="23" t="n">
         <v>0</v>
       </c>
       <c r="G181" s="9" t="n">
@@ -6731,22 +6745,22 @@
       <c r="Z181" s="2"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="20" t="s">
+      <c r="A182" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B182" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C182" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D182" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E182" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F182" s="21" t="n">
+      <c r="B182" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C182" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" s="23" t="n">
         <v>0</v>
       </c>
       <c r="G182" s="9" t="n">
@@ -6769,22 +6783,22 @@
       <c r="Z182" s="2"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="20" t="s">
+      <c r="A183" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B183" s="21" t="n">
+      <c r="B183" s="23" t="n">
         <v>27.317</v>
       </c>
-      <c r="C183" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D183" s="21" t="n">
+      <c r="C183" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" s="23" t="n">
         <v>-0.625</v>
       </c>
-      <c r="E183" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F183" s="21" t="n">
+      <c r="E183" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" s="23" t="n">
         <v>0</v>
       </c>
       <c r="G183" s="9" t="n">
@@ -6807,16 +6821,16 @@
       <c r="Z183" s="2"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="20" t="s">
+      <c r="A184" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B184" s="21" t="n">
+      <c r="B184" s="23" t="n">
         <v>9.538</v>
       </c>
-      <c r="C184" s="20"/>
-      <c r="D184" s="20"/>
-      <c r="E184" s="20"/>
-      <c r="F184" s="20"/>
+      <c r="C184" s="22"/>
+      <c r="D184" s="22"/>
+      <c r="E184" s="22"/>
+      <c r="F184" s="22"/>
       <c r="G184" s="2"/>
       <c r="L184" s="2"/>
       <c r="M184" s="2"/>
@@ -6835,20 +6849,20 @@
       <c r="Z184" s="2"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="20"/>
-      <c r="B185" s="20" t="s">
+      <c r="A185" s="22"/>
+      <c r="B185" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C185" s="20" t="s">
+      <c r="C185" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D185" s="20" t="s">
+      <c r="D185" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E185" s="20" t="s">
+      <c r="E185" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F185" s="20" t="s">
+      <c r="F185" s="22" t="s">
         <v>36</v>
       </c>
       <c r="G185" s="2" t="s">
@@ -6874,25 +6888,25 @@
       <c r="Z185" s="2"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="20" t="s">
+      <c r="A186" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B186" s="22" t="n">
+      <c r="B186" s="24" t="n">
         <v>1.032E-005</v>
       </c>
-      <c r="C186" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D186" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E186" s="22" t="n">
+      <c r="C186" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" s="24" t="n">
         <v>3.393E-007</v>
       </c>
-      <c r="F186" s="22" t="n">
+      <c r="F186" s="24" t="n">
         <v>-3.583E-007</v>
       </c>
-      <c r="G186" s="22" t="n">
+      <c r="G186" s="24" t="n">
         <v>1.021E-005</v>
       </c>
       <c r="J186" s="2"/>
@@ -6914,16 +6928,16 @@
       <c r="Z186" s="2"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="20" t="s">
+      <c r="A187" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B187" s="23" t="s">
+      <c r="B187" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C187" s="20"/>
-      <c r="D187" s="20"/>
-      <c r="E187" s="24"/>
-      <c r="F187" s="20"/>
+      <c r="C187" s="22"/>
+      <c r="D187" s="22"/>
+      <c r="E187" s="26"/>
+      <c r="F187" s="22"/>
       <c r="G187" s="2"/>
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
@@ -6950,10 +6964,10 @@
       <c r="B188" s="14" t="n">
         <v>2.54E-006</v>
       </c>
-      <c r="C188" s="20"/>
-      <c r="D188" s="20"/>
-      <c r="E188" s="24"/>
-      <c r="F188" s="20"/>
+      <c r="C188" s="22"/>
+      <c r="D188" s="22"/>
+      <c r="E188" s="26"/>
+      <c r="F188" s="22"/>
       <c r="G188" s="2"/>
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
@@ -6974,16 +6988,16 @@
       <c r="Z188" s="2"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="25" t="s">
+      <c r="A189" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B189" s="23" t="s">
+      <c r="B189" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C189" s="25"/>
-      <c r="D189" s="25"/>
-      <c r="E189" s="25"/>
-      <c r="F189" s="25"/>
+      <c r="C189" s="27"/>
+      <c r="D189" s="27"/>
+      <c r="E189" s="27"/>
+      <c r="F189" s="27"/>
       <c r="J189" s="2"/>
       <c r="K189" s="2"/>
       <c r="L189" s="2"/>
@@ -7003,16 +7017,16 @@
       <c r="Z189" s="2"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="25" t="s">
+      <c r="A190" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B190" s="21" t="n">
+      <c r="B190" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="C190" s="25"/>
-      <c r="D190" s="25"/>
-      <c r="E190" s="25"/>
-      <c r="F190" s="25"/>
+      <c r="C190" s="27"/>
+      <c r="D190" s="27"/>
+      <c r="E190" s="27"/>
+      <c r="F190" s="27"/>
       <c r="J190" s="2"/>
       <c r="K190" s="2"/>
       <c r="L190" s="2"/>
@@ -7032,16 +7046,16 @@
       <c r="Z190" s="2"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="25" t="s">
+      <c r="A191" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B191" s="21" t="n">
+      <c r="B191" s="23" t="n">
         <v>2.64</v>
       </c>
-      <c r="C191" s="25"/>
-      <c r="D191" s="25"/>
-      <c r="E191" s="25"/>
-      <c r="F191" s="25"/>
+      <c r="C191" s="27"/>
+      <c r="D191" s="27"/>
+      <c r="E191" s="27"/>
+      <c r="F191" s="27"/>
       <c r="I191" s="12" t="s">
         <v>115</v>
       </c>
@@ -7064,22 +7078,22 @@
       <c r="Z191" s="2"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="25" t="s">
+      <c r="A192" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B192" s="21" t="n">
+      <c r="B192" s="23" t="n">
         <v>-0.0351</v>
       </c>
-      <c r="C192" s="21" t="n">
+      <c r="C192" s="23" t="n">
         <v>0.1081</v>
       </c>
-      <c r="D192" s="21" t="n">
+      <c r="D192" s="23" t="n">
         <v>-0.1479</v>
       </c>
-      <c r="E192" s="21" t="n">
+      <c r="E192" s="23" t="n">
         <v>-0.1421</v>
       </c>
-      <c r="F192" s="21" t="n">
+      <c r="F192" s="23" t="n">
         <v>0.1092</v>
       </c>
       <c r="I192" s="12" t="s">
@@ -7104,22 +7118,22 @@
       <c r="Z192" s="2"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="25" t="s">
+      <c r="A193" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B193" s="21" t="n">
+      <c r="B193" s="23" t="n">
         <v>0.1774</v>
       </c>
-      <c r="C193" s="21" t="n">
+      <c r="C193" s="23" t="n">
         <v>-0.3766</v>
       </c>
-      <c r="D193" s="21" t="n">
+      <c r="D193" s="23" t="n">
         <v>-0.0164</v>
       </c>
-      <c r="E193" s="21" t="n">
+      <c r="E193" s="23" t="n">
         <v>0.0261</v>
       </c>
-      <c r="F193" s="21" t="n">
+      <c r="F193" s="23" t="n">
         <v>0.0396</v>
       </c>
       <c r="I193" s="12" t="s">
@@ -7525,7 +7539,7 @@
       <c r="Z204" s="2"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="16" t="s">
+      <c r="A205" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B205" s="9" t="s">
@@ -7550,7 +7564,7 @@
       <c r="Z205" s="2"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="16" t="s">
+      <c r="A206" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B206" s="9" t="n">
@@ -7575,7 +7589,7 @@
       <c r="Z206" s="2"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="16" t="s">
+      <c r="A207" s="17" t="s">
         <v>114</v>
       </c>
       <c r="B207" s="9" t="n">
@@ -7600,7 +7614,7 @@
       <c r="Z207" s="2"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="16" t="s">
+      <c r="A208" s="17" t="s">
         <v>116</v>
       </c>
       <c r="B208" s="9" t="n">
@@ -7638,7 +7652,7 @@
       <c r="Z208" s="2"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="16" t="s">
+      <c r="A209" s="17" t="s">
         <v>118</v>
       </c>
       <c r="B209" s="9" t="n">
@@ -8117,7 +8131,7 @@
       <c r="Z223" s="2"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="16" t="s">
+      <c r="A224" s="17" t="s">
         <v>129</v>
       </c>
       <c r="B224" s="9" t="n">
@@ -8141,7 +8155,7 @@
       <c r="Z224" s="2"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="16" t="s">
+      <c r="A225" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B225" s="9" t="n">
@@ -8165,7 +8179,7 @@
       <c r="Z225" s="2"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A226" s="16" t="s">
+      <c r="A226" s="17" t="s">
         <v>133</v>
       </c>
       <c r="B226" s="9" t="n">
@@ -8189,7 +8203,7 @@
       <c r="Z226" s="2"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="16" t="s">
+      <c r="A227" s="17" t="s">
         <v>135</v>
       </c>
       <c r="B227" s="9" t="n">

</xml_diff>